<commit_message>
add data training confussion matrix
</commit_message>
<xml_diff>
--- a/data_penumpang.xlsx
+++ b/data_penumpang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookairm2/R/desicisionTreeC50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D4B7A7-7685-1446-ACF8-61425E903C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9910DDC-D6F7-B648-A611-82BA7AEA11B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{A07AD527-ABE1-47DC-93DF-9243556C13F3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="514">
   <si>
     <t>ID Penumpang</t>
   </si>
@@ -8997,7 +8997,7 @@
   <dimension ref="A1:F492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F1" sqref="F1:F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9018,9 +9018,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -9038,9 +9036,7 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -9058,9 +9054,7 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -9078,9 +9072,7 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -9098,9 +9090,7 @@
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -9118,9 +9108,7 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -9138,9 +9126,7 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -9158,9 +9144,7 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -9178,9 +9162,7 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -9198,9 +9180,7 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -9218,9 +9198,7 @@
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -9238,9 +9216,7 @@
       <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -9258,9 +9234,7 @@
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -9278,9 +9252,7 @@
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -9298,9 +9270,7 @@
       <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -9318,9 +9288,7 @@
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -9338,9 +9306,7 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -9358,9 +9324,7 @@
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -9378,9 +9342,7 @@
       <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -9398,9 +9360,7 @@
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -9418,9 +9378,7 @@
       <c r="E21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -9438,9 +9396,7 @@
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -9458,9 +9414,7 @@
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -9478,9 +9432,7 @@
       <c r="E24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -9498,9 +9450,7 @@
       <c r="E25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -9518,9 +9468,7 @@
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -9538,9 +9486,7 @@
       <c r="E27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -9558,9 +9504,7 @@
       <c r="E28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -9578,9 +9522,7 @@
       <c r="E29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -9598,9 +9540,7 @@
       <c r="E30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -9618,9 +9558,7 @@
       <c r="E31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -9638,9 +9576,7 @@
       <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -9658,9 +9594,7 @@
       <c r="E33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -9678,9 +9612,7 @@
       <c r="E34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -9698,9 +9630,7 @@
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -9718,9 +9648,7 @@
       <c r="E36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="2">
-        <v>0</v>
-      </c>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -9738,9 +9666,7 @@
       <c r="E37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="2">
-        <v>1</v>
-      </c>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -9758,9 +9684,7 @@
       <c r="E38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -9778,9 +9702,7 @@
       <c r="E39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="2">
-        <v>0</v>
-      </c>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
@@ -9798,9 +9720,7 @@
       <c r="E40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -9818,9 +9738,7 @@
       <c r="E41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
+      <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -9838,9 +9756,7 @@
       <c r="E42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="2">
-        <v>1</v>
-      </c>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -9858,9 +9774,7 @@
       <c r="E43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="2">
-        <v>0</v>
-      </c>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -9878,9 +9792,7 @@
       <c r="E44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -9898,9 +9810,7 @@
       <c r="E45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="2">
-        <v>0</v>
-      </c>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -9918,9 +9828,7 @@
       <c r="E46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F46" s="2">
-        <v>1</v>
-      </c>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -9938,9 +9846,7 @@
       <c r="E47" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="2">
-        <v>0</v>
-      </c>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -9958,9 +9864,7 @@
       <c r="E48" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="2">
-        <v>1</v>
-      </c>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -9978,9 +9882,7 @@
       <c r="E49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="2">
-        <v>1</v>
-      </c>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
@@ -9998,9 +9900,7 @@
       <c r="E50" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="2">
-        <v>0</v>
-      </c>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
@@ -10018,9 +9918,7 @@
       <c r="E51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="2">
-        <v>1</v>
-      </c>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
@@ -10038,9 +9936,7 @@
       <c r="E52" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="2">
-        <v>0</v>
-      </c>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
@@ -10058,9 +9954,7 @@
       <c r="E53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="2">
-        <v>1</v>
-      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
@@ -10078,9 +9972,7 @@
       <c r="E54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="2">
-        <v>1</v>
-      </c>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
@@ -10098,9 +9990,7 @@
       <c r="E55" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F55" s="2">
-        <v>1</v>
-      </c>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
@@ -10118,9 +10008,7 @@
       <c r="E56" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="2">
-        <v>0</v>
-      </c>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -10138,9 +10026,7 @@
       <c r="E57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="2">
-        <v>0</v>
-      </c>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
@@ -10158,9 +10044,7 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="2">
-        <v>1</v>
-      </c>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
@@ -10178,9 +10062,7 @@
       <c r="E59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="2">
-        <v>1</v>
-      </c>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
@@ -10198,9 +10080,7 @@
       <c r="E60" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="2">
-        <v>1</v>
-      </c>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
@@ -10218,9 +10098,7 @@
       <c r="E61" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="2">
-        <v>0</v>
-      </c>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
@@ -10238,9 +10116,7 @@
       <c r="E62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="2">
-        <v>1</v>
-      </c>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
@@ -10258,9 +10134,7 @@
       <c r="E63" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="2">
-        <v>1</v>
-      </c>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
@@ -10278,9 +10152,7 @@
       <c r="E64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="2">
-        <v>0</v>
-      </c>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
@@ -10298,9 +10170,7 @@
       <c r="E65" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="2">
-        <v>0</v>
-      </c>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
@@ -10318,9 +10188,7 @@
       <c r="E66" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="2">
-        <v>0</v>
-      </c>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
@@ -10338,9 +10206,7 @@
       <c r="E67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F67" s="2">
-        <v>1</v>
-      </c>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
@@ -10358,9 +10224,7 @@
       <c r="E68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="2">
-        <v>1</v>
-      </c>
+      <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -10378,9 +10242,7 @@
       <c r="E69" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="2">
-        <v>1</v>
-      </c>
+      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
@@ -10398,9 +10260,7 @@
       <c r="E70" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="2">
-        <v>1</v>
-      </c>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -10418,9 +10278,7 @@
       <c r="E71" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="2">
-        <v>1</v>
-      </c>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
@@ -10438,9 +10296,7 @@
       <c r="E72" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="2">
-        <v>0</v>
-      </c>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
@@ -10458,9 +10314,7 @@
       <c r="E73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="2">
-        <v>1</v>
-      </c>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
@@ -10478,9 +10332,7 @@
       <c r="E74" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F74" s="2">
-        <v>0</v>
-      </c>
+      <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
@@ -10498,9 +10350,7 @@
       <c r="E75" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F75" s="2">
-        <v>1</v>
-      </c>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
@@ -10518,9 +10368,7 @@
       <c r="E76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F76" s="2">
-        <v>1</v>
-      </c>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
@@ -10538,9 +10386,7 @@
       <c r="E77" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F77" s="2">
-        <v>1</v>
-      </c>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
@@ -10558,9 +10404,7 @@
       <c r="E78" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F78" s="2">
-        <v>0</v>
-      </c>
+      <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
@@ -10578,9 +10422,7 @@
       <c r="E79" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F79" s="2">
-        <v>0</v>
-      </c>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
@@ -10598,9 +10440,7 @@
       <c r="E80" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F80" s="2">
-        <v>0</v>
-      </c>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
@@ -10618,9 +10458,7 @@
       <c r="E81" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F81" s="2">
-        <v>1</v>
-      </c>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
@@ -10638,9 +10476,7 @@
       <c r="E82" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F82" s="2">
-        <v>0</v>
-      </c>
+      <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
@@ -10658,9 +10494,7 @@
       <c r="E83" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F83" s="2">
-        <v>1</v>
-      </c>
+      <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
@@ -10678,9 +10512,7 @@
       <c r="E84" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F84" s="2">
-        <v>1</v>
-      </c>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
@@ -10698,9 +10530,7 @@
       <c r="E85" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F85" s="2">
-        <v>0</v>
-      </c>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
@@ -10718,9 +10548,7 @@
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F86" s="2">
-        <v>1</v>
-      </c>
+      <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
@@ -10738,9 +10566,7 @@
       <c r="E87" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F87" s="2">
-        <v>0</v>
-      </c>
+      <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
@@ -10758,9 +10584,7 @@
       <c r="E88" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F88" s="2">
-        <v>1</v>
-      </c>
+      <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
@@ -10778,9 +10602,7 @@
       <c r="E89" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F89" s="2">
-        <v>1</v>
-      </c>
+      <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
@@ -10798,9 +10620,7 @@
       <c r="E90" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F90" s="2">
-        <v>1</v>
-      </c>
+      <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
@@ -10818,9 +10638,7 @@
       <c r="E91" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F91" s="2">
-        <v>1</v>
-      </c>
+      <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
@@ -10838,9 +10656,7 @@
       <c r="E92" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F92" s="2">
-        <v>0</v>
-      </c>
+      <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
@@ -10858,9 +10674,7 @@
       <c r="E93" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F93" s="2">
-        <v>0</v>
-      </c>
+      <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
@@ -10878,9 +10692,7 @@
       <c r="E94" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F94" s="2">
-        <v>1</v>
-      </c>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
@@ -10898,9 +10710,7 @@
       <c r="E95" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F95" s="2">
-        <v>0</v>
-      </c>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
@@ -10918,9 +10728,7 @@
       <c r="E96" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F96" s="2">
-        <v>0</v>
-      </c>
+      <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
@@ -10938,9 +10746,7 @@
       <c r="E97" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F97" s="2">
-        <v>1</v>
-      </c>
+      <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
@@ -10958,9 +10764,7 @@
       <c r="E98" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F98" s="2">
-        <v>0</v>
-      </c>
+      <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
@@ -10978,9 +10782,7 @@
       <c r="E99" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F99" s="2">
-        <v>1</v>
-      </c>
+      <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
@@ -10998,9 +10800,7 @@
       <c r="E100" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F100" s="2">
-        <v>1</v>
-      </c>
+      <c r="F100" s="2"/>
     </row>
     <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
@@ -11018,9 +10818,7 @@
       <c r="E101" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F101" s="2">
-        <v>0</v>
-      </c>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
@@ -11038,9 +10836,7 @@
       <c r="E102" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F102" s="2">
-        <v>1</v>
-      </c>
+      <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
@@ -11058,9 +10854,7 @@
       <c r="E103" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F103" s="2">
-        <v>0</v>
-      </c>
+      <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
@@ -11078,9 +10872,7 @@
       <c r="E104" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="2">
-        <v>0</v>
-      </c>
+      <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
@@ -11098,9 +10890,7 @@
       <c r="E105" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F105" s="2">
-        <v>1</v>
-      </c>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
@@ -11118,9 +10908,7 @@
       <c r="E106" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F106" s="2">
-        <v>1</v>
-      </c>
+      <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
@@ -11138,9 +10926,7 @@
       <c r="E107" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F107" s="2">
-        <v>0</v>
-      </c>
+      <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
@@ -11158,9 +10944,7 @@
       <c r="E108" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F108" s="2">
-        <v>1</v>
-      </c>
+      <c r="F108" s="2"/>
     </row>
     <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
@@ -11178,9 +10962,7 @@
       <c r="E109" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F109" s="2">
-        <v>1</v>
-      </c>
+      <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
@@ -11198,9 +10980,7 @@
       <c r="E110" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="2">
-        <v>1</v>
-      </c>
+      <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
@@ -11218,9 +10998,7 @@
       <c r="E111" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F111" s="2">
-        <v>0</v>
-      </c>
+      <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
@@ -11238,9 +11016,7 @@
       <c r="E112" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F112" s="2">
-        <v>1</v>
-      </c>
+      <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
@@ -11258,9 +11034,7 @@
       <c r="E113" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F113" s="2">
-        <v>0</v>
-      </c>
+      <c r="F113" s="2"/>
     </row>
     <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
@@ -11278,9 +11052,7 @@
       <c r="E114" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F114" s="2">
-        <v>0</v>
-      </c>
+      <c r="F114" s="2"/>
     </row>
     <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
@@ -11298,9 +11070,7 @@
       <c r="E115" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F115" s="2">
-        <v>1</v>
-      </c>
+      <c r="F115" s="2"/>
     </row>
     <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
@@ -11318,9 +11088,7 @@
       <c r="E116" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F116" s="2">
-        <v>0</v>
-      </c>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
@@ -11338,9 +11106,7 @@
       <c r="E117" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F117" s="2">
-        <v>1</v>
-      </c>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
@@ -11358,9 +11124,7 @@
       <c r="E118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F118" s="2">
-        <v>1</v>
-      </c>
+      <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
@@ -11378,9 +11142,7 @@
       <c r="E119" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F119" s="2">
-        <v>1</v>
-      </c>
+      <c r="F119" s="2"/>
     </row>
     <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
@@ -11398,9 +11160,7 @@
       <c r="E120" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F120" s="2">
-        <v>1</v>
-      </c>
+      <c r="F120" s="2"/>
     </row>
     <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
@@ -11418,9 +11178,7 @@
       <c r="E121" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F121" s="2">
-        <v>1</v>
-      </c>
+      <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
@@ -11438,9 +11196,7 @@
       <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="2">
-        <v>1</v>
-      </c>
+      <c r="F122" s="2"/>
     </row>
     <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
@@ -11458,9 +11214,7 @@
       <c r="E123" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F123" s="2">
-        <v>0</v>
-      </c>
+      <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
@@ -11478,9 +11232,7 @@
       <c r="E124" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F124" s="2">
-        <v>1</v>
-      </c>
+      <c r="F124" s="2"/>
     </row>
     <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
@@ -11498,9 +11250,7 @@
       <c r="E125" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F125" s="2">
-        <v>1</v>
-      </c>
+      <c r="F125" s="2"/>
     </row>
     <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
@@ -11518,9 +11268,7 @@
       <c r="E126" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F126" s="2">
-        <v>1</v>
-      </c>
+      <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
@@ -11538,9 +11286,7 @@
       <c r="E127" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F127" s="2">
-        <v>0</v>
-      </c>
+      <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
@@ -11558,9 +11304,7 @@
       <c r="E128" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F128" s="2">
-        <v>0</v>
-      </c>
+      <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
@@ -11578,9 +11322,7 @@
       <c r="E129" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F129" s="2">
-        <v>0</v>
-      </c>
+      <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
@@ -11598,9 +11340,7 @@
       <c r="E130" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F130" s="2">
-        <v>1</v>
-      </c>
+      <c r="F130" s="2"/>
     </row>
     <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
@@ -11618,9 +11358,7 @@
       <c r="E131" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F131" s="2">
-        <v>1</v>
-      </c>
+      <c r="F131" s="2"/>
     </row>
     <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
@@ -11638,9 +11376,7 @@
       <c r="E132" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F132" s="2">
-        <v>1</v>
-      </c>
+      <c r="F132" s="2"/>
     </row>
     <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
@@ -11658,9 +11394,7 @@
       <c r="E133" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F133" s="2">
-        <v>1</v>
-      </c>
+      <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
@@ -11678,9 +11412,7 @@
       <c r="E134" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F134" s="2">
-        <v>0</v>
-      </c>
+      <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
@@ -11698,9 +11430,7 @@
       <c r="E135" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F135" s="2">
-        <v>1</v>
-      </c>
+      <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
@@ -11718,9 +11448,7 @@
       <c r="E136" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F136" s="2">
-        <v>1</v>
-      </c>
+      <c r="F136" s="2"/>
     </row>
     <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
@@ -11738,9 +11466,7 @@
       <c r="E137" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F137" s="2">
-        <v>0</v>
-      </c>
+      <c r="F137" s="2"/>
     </row>
     <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
@@ -11758,9 +11484,7 @@
       <c r="E138" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F138" s="2">
-        <v>0</v>
-      </c>
+      <c r="F138" s="2"/>
     </row>
     <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
@@ -11778,9 +11502,7 @@
       <c r="E139" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F139" s="2">
-        <v>1</v>
-      </c>
+      <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
@@ -11798,9 +11520,7 @@
       <c r="E140" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F140" s="2">
-        <v>0</v>
-      </c>
+      <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
@@ -11818,9 +11538,7 @@
       <c r="E141" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F141" s="2">
-        <v>0</v>
-      </c>
+      <c r="F141" s="2"/>
     </row>
     <row r="142" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
@@ -11838,9 +11556,7 @@
       <c r="E142" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F142" s="2">
-        <v>0</v>
-      </c>
+      <c r="F142" s="2"/>
     </row>
     <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
@@ -11858,9 +11574,7 @@
       <c r="E143" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F143" s="2">
-        <v>1</v>
-      </c>
+      <c r="F143" s="2"/>
     </row>
     <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
@@ -11878,9 +11592,7 @@
       <c r="E144" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F144" s="2">
-        <v>1</v>
-      </c>
+      <c r="F144" s="2"/>
     </row>
     <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
@@ -11898,9 +11610,7 @@
       <c r="E145" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F145" s="2">
-        <v>0</v>
-      </c>
+      <c r="F145" s="2"/>
     </row>
     <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
@@ -11918,9 +11628,7 @@
       <c r="E146" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F146" s="2">
-        <v>0</v>
-      </c>
+      <c r="F146" s="2"/>
     </row>
     <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
@@ -11938,9 +11646,7 @@
       <c r="E147" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F147" s="2">
-        <v>1</v>
-      </c>
+      <c r="F147" s="2"/>
     </row>
     <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
@@ -11958,9 +11664,7 @@
       <c r="E148" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F148" s="2">
-        <v>1</v>
-      </c>
+      <c r="F148" s="2"/>
     </row>
     <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
@@ -11978,9 +11682,7 @@
       <c r="E149" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F149" s="2">
-        <v>0</v>
-      </c>
+      <c r="F149" s="2"/>
     </row>
     <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
@@ -11998,9 +11700,7 @@
       <c r="E150" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F150" s="2">
-        <v>1</v>
-      </c>
+      <c r="F150" s="2"/>
     </row>
     <row r="151" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
@@ -12018,9 +11718,7 @@
       <c r="E151" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F151" s="2">
-        <v>0</v>
-      </c>
+      <c r="F151" s="2"/>
     </row>
     <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>

</xml_diff>